<commit_message>
Se hacen nuevas validaciones
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="58">
   <si>
     <t>Ficha</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t>VERDADERO</t>
+  </si>
+  <si>
+    <t>FALSO - Documento sólo en Instructores</t>
+  </si>
+  <si>
+    <t>FALSO - Documento sólo en Sofía</t>
   </si>
   <si>
     <t>FALSO - Discrepancia en Nombre: Instructores (GLORIA YENNY CASTILLO ESPAÑAS) vs Sofía (GLORIA YENNY CASTILLO ESPAÑA)</t>
@@ -539,7 +545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -861,38 +867,17 @@
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10">
-        <v>3031278</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
       <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="H10">
-        <v>25018849</v>
-      </c>
       <c r="I10" t="s">
         <v>42</v>
       </c>
-      <c r="J10" t="s">
-        <v>42</v>
-      </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -908,26 +893,17 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
       <c r="H11">
-        <v>31642764</v>
-      </c>
-      <c r="I11" t="s">
-        <v>43</v>
+        <v>250188492</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -950,16 +926,16 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H12">
-        <v>31863992</v>
+        <v>31642764</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
         <v>53</v>
@@ -985,16 +961,16 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13">
-        <v>32731171</v>
+        <v>31863992</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
         <v>53</v>
@@ -1020,19 +996,19 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H14">
-        <v>36380685</v>
+        <v>32731171</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1055,19 +1031,19 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15">
-        <v>38553002</v>
+        <v>36380685</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="K15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1090,16 +1066,16 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H16">
-        <v>42057870</v>
+        <v>38553002</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K16" t="s">
         <v>53</v>
@@ -1125,16 +1101,16 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17">
-        <v>66655884</v>
+        <v>42057870</v>
       </c>
       <c r="I17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K17" t="s">
         <v>53</v>
@@ -1157,22 +1133,22 @@
         <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18">
-        <v>66756576</v>
+        <v>66655884</v>
       </c>
       <c r="I18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1192,21 +1168,56 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19">
+        <v>66756576</v>
+      </c>
+      <c r="I19" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20">
+        <v>3031278</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
         <v>33</v>
       </c>
-      <c r="H19">
+      <c r="H20">
         <v>66767235</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I20" t="s">
         <v>51</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>51</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K20" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se hace nuevo login
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="60">
   <si>
     <t>Ficha</t>
   </si>
@@ -82,13 +82,13 @@
     <t>16698345</t>
   </si>
   <si>
-    <t>16739327</t>
+    <t>167393272</t>
   </si>
   <si>
     <t>18464762</t>
   </si>
   <si>
-    <t>25018849</t>
+    <t>250188492</t>
   </si>
   <si>
     <t>31642764</t>
@@ -97,7 +97,7 @@
     <t>31863992</t>
   </si>
   <si>
-    <t>32731171</t>
+    <t>327311712</t>
   </si>
   <si>
     <t>36380685</t>
@@ -139,49 +139,55 @@
     <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
   </si>
   <si>
+    <t>LUIS EDUARDO OLIVEROS RAMIRES</t>
+  </si>
+  <si>
+    <t>NORA MARIA BLANDON SERNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+  </si>
+  <si>
+    <t>ALBA INES ZULETA JARAMILLO</t>
+  </si>
+  <si>
+    <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+  </si>
+  <si>
+    <t>GLORIA YENNY CASTILLO ESPAÑAS</t>
+  </si>
+  <si>
+    <t>PAOLA ANDREA CASTILLO ALZATE</t>
+  </si>
+  <si>
+    <t>MARTHA LUCIA ALZATE GOMEZ</t>
+  </si>
+  <si>
+    <t>MARIA DEL CARMEN CERON BEDOYA</t>
+  </si>
+  <si>
+    <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+  </si>
+  <si>
+    <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
+  </si>
+  <si>
     <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
   </si>
   <si>
-    <t>NORA MARIA BLANDON SERNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
-  </si>
-  <si>
-    <t>ALBA INES ZULETA JARAMILLO</t>
-  </si>
-  <si>
-    <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
-  </si>
-  <si>
-    <t>GLORIA YENNY CASTILLO ESPAÑAS</t>
-  </si>
-  <si>
-    <t>PAOLA ANDREA CASTILLO ALZATE</t>
-  </si>
-  <si>
-    <t>MARTHA LUCIA ALZATE GOMEZ</t>
-  </si>
-  <si>
-    <t>MARIA DEL CARMEN CERON BEDOYA</t>
-  </si>
-  <si>
-    <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
-  </si>
-  <si>
-    <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
-  </si>
-  <si>
     <t>GLORIA YENNY CASTILLO ESPAÑA</t>
   </si>
   <si>
     <t>VERDADERO</t>
   </si>
   <si>
+    <t>FALSO - Documento sólo en Sofía</t>
+  </si>
+  <si>
     <t>FALSO - Documento sólo en Instructores</t>
   </si>
   <si>
-    <t>FALSO - Documento sólo en Sofía</t>
+    <t>FALSO - Discrepancia en Nombre: Instructores (LUIS EDUARDO OLIVEROS RAMIRES) vs Sofía (LUIS EDUARDO OLIVEROS RAMIREZ)</t>
   </si>
   <si>
     <t>FALSO - Discrepancia en Nombre: Instructores (GLORIA YENNY CASTILLO ESPAÑAS) vs Sofía (GLORIA YENNY CASTILLO ESPAÑA)</t>
@@ -545,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -618,7 +624,7 @@
         <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -653,7 +659,7 @@
         <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -688,7 +694,7 @@
         <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -723,7 +729,7 @@
         <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -758,7 +764,7 @@
         <v>38</v>
       </c>
       <c r="K6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -793,7 +799,7 @@
         <v>39</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -809,75 +815,66 @@
       <c r="D8" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
       <c r="F8" t="s">
         <v>14</v>
-      </c>
-      <c r="G8" t="s">
-        <v>22</v>
       </c>
       <c r="H8">
         <v>16739327</v>
       </c>
-      <c r="I8" t="s">
-        <v>40</v>
-      </c>
       <c r="J8" t="s">
         <v>40</v>
       </c>
       <c r="K8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9">
-        <v>3031278</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
       <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>3031278</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
         <v>23</v>
       </c>
-      <c r="H9">
+      <c r="H10">
         <v>18464762</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>41</v>
       </c>
-      <c r="J9" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>42</v>
+      <c r="J10" t="s">
+        <v>52</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -893,17 +890,26 @@
       <c r="D11" t="s">
         <v>13</v>
       </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
       <c r="F11" t="s">
         <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
       </c>
       <c r="H11">
         <v>250188492</v>
       </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
       <c r="J11" t="s">
         <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -938,7 +944,7 @@
         <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -973,7 +979,7 @@
         <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -989,58 +995,28 @@
       <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
       <c r="F14" t="s">
         <v>14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>27</v>
       </c>
       <c r="H14">
         <v>32731171</v>
       </c>
-      <c r="I14" t="s">
-        <v>45</v>
-      </c>
       <c r="J14" t="s">
         <v>45</v>
       </c>
       <c r="K14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15">
-        <v>3031278</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
       <c r="G15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15">
-        <v>36380685</v>
+        <v>27</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
-      </c>
-      <c r="J15" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K15" t="s">
         <v>56</v>
@@ -1066,19 +1042,19 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16">
-        <v>38553002</v>
+        <v>36380685</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="K16" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1101,19 +1077,19 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H17">
-        <v>42057870</v>
+        <v>38553002</v>
       </c>
       <c r="I17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1136,19 +1112,19 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18">
-        <v>66655884</v>
+        <v>42057870</v>
       </c>
       <c r="I18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K18" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1168,22 +1144,22 @@
         <v>14</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H19">
-        <v>66756576</v>
+        <v>66655884</v>
       </c>
       <c r="I19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1203,22 +1179,57 @@
         <v>14</v>
       </c>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20">
+        <v>66756576</v>
+      </c>
+      <c r="I20" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21">
+        <v>3031278</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
         <v>33</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>66767235</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
         <v>51</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>51</v>
       </c>
-      <c r="K20" t="s">
-        <v>53</v>
+      <c r="K21" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se empieza hacer el tercer modulo
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -879,14 +879,29 @@
           <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>167393272</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>16739327</t>
+          <t>167393272</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -896,29 +911,62 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Sofía</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>167393272</t>
+          <t>18464762</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>18464762</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
+          <t>LUIS EDUARDO OLIVEROS RAMIRES</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (LUIS EDUARDO OLIVEROS RAMIRES) vs Sofía (LUIS EDUARDO OLIVEROS RAMIREZ)</t>
         </is>
       </c>
     </row>
@@ -953,27 +1001,27 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>18464762</t>
+          <t>250188492</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>18464762</t>
+          <t>250188492</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIRES</t>
+          <t>NORA MARIA BLANDON SERNA</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
+          <t>NORA MARIA BLANDON SERNA</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (LUIS EDUARDO OLIVEROS RAMIRES) vs Sofía (LUIS EDUARDO OLIVEROS RAMIREZ)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1008,22 +1056,22 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>250188492</t>
+          <t>31642764</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>250188492</t>
+          <t>31642764</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>NORA MARIA BLANDON SERNA</t>
+          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>NORA MARIA BLANDON SERNA</t>
+          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
@@ -1063,22 +1111,22 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>31642764</t>
+          <t>31863992</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>31642764</t>
+          <t>31863992</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+          <t>ALBA INES ZULETA JARAMILLO</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+          <t>ALBA INES ZULETA JARAMILLO</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1118,22 +1166,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>31863992</t>
+          <t>327311712</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>31863992</t>
+          <t>327311712</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
+          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
+          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -1161,46 +1209,94 @@
           <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>36380685</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>32731171</t>
+          <t>36380685</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Sofía</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>327311712</t>
+          <t>38553002</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>38553002</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>PAOLA ANDREA CASTILLO ALZATE</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1235,22 +1331,22 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>36380685</t>
+          <t>42057870</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>36380685</t>
+          <t>42057870</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
+          <t>MARTHA LUCIA ALZATE GOMEZ</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
+          <t>MARTHA LUCIA ALZATE GOMEZ</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -1290,22 +1386,22 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>38553002</t>
+          <t>66655884</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>38553002</t>
+          <t>66655884</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>MARIA DEL CARMEN CERON BEDOYA</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>MARIA DEL CARMEN CERON BEDOYA</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -1340,32 +1436,32 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>42057870</t>
+          <t>66756576</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>42057870</t>
+          <t>66756576</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
+          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
+          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Discrepancia en Tipo de Documento: Instructores (CC) vs Sofía (TI)</t>
         </is>
       </c>
     </row>
@@ -1400,135 +1496,25 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>66655884</t>
+          <t>66767235</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>66655884</t>
+          <t>66767235</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
+          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
+          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
-        <is>
-          <t>VERDADERO</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>66756576</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>66756576</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>FALSO - Discrepancia en Tipo de Documento: Instructores (CC) vs Sofía (TI)</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>66767235</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>66767235</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
         <is>
           <t>VERDADERO</t>
         </is>

</xml_diff>

<commit_message>
Funcionan los dos archivos (INSTRU) vs (SOFIA)
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,14 @@
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="41" customWidth="1" min="4" max="4"/>
+    <col width="71" customWidth="1" min="4" max="4"/>
     <col width="29" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
     <col width="28" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
-    <col width="36" customWidth="1" min="9" max="9"/>
-    <col width="36" customWidth="1" min="10" max="10"/>
-    <col width="119" customWidth="1" min="11" max="11"/>
+    <col width="39" customWidth="1" min="9" max="9"/>
+    <col width="31" customWidth="1" min="10" max="10"/>
+    <col width="116" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -516,7 +516,7 @@
       </c>
       <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Nombre Aprendiz Instructores</t>
+          <t>Nombre Aprendiz Instructores Consulta</t>
         </is>
       </c>
       <c r="J1" s="2" t="inlineStr">
@@ -531,393 +531,162 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1005551692</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>1005551692</t>
+          <t>1001779425</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>ZOILA LUZ ALVAREZ CALDERON</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>ZOILA LUZ ALVAREZ CALDERON</t>
+          <t>SEBASTIANJIMENEZMAGALLANES</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1010141404</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>1010141404</t>
+          <t>1002921910</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>LIZETH VANESSA PEDREROS ARANGO</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>LIZETH VANESSA PEDREROS ARANGO</t>
+          <t>ESTEFANNYGISELLAMUÑOZBARCO</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1051821219</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1051821219</t>
+          <t>1003237027</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>CLAUDIA PATRICIA GRAVIER CALDERON</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>CLAUDIA PATRICIA GRAVIER CALDERON</t>
+          <t>CLAUDIAELENARESTREPOARANGO</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1116242829</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>1116242829</t>
+          <t>1003244042</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>LAURA MARCELA QUINTERO SANCHEZ</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>LAURA MARCELA QUINTERO SANCHEZ</t>
+          <t>DUBYSTATIANABLANQUICETTMEJIA</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1130643841</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>1130643841</t>
+          <t>1003764743</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
+          <t>NEWMANESTIBENESCOBARCERON</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>16698345</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>16698345</t>
+          <t>1004999377</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>OMAR URIEL PATIÑO TORRES</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>OMAR URIEL PATIÑO TORRES</t>
+          <t>ALIXVALENTINAANGARITAANGARITA</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>167393272</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>167393272</t>
+          <t>1005870821</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
+          <t>MICHAELSTEVENCAMACHOACEVEDO</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3031278</v>
+        <v>3127639</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -931,7 +700,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -946,198 +715,99 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>18464762</t>
+          <t>1007514084</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>18464762</t>
+          <t>1007514084</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIRES</t>
+          <t>MARYURIAVENDAÑOBADILLO</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
+          <t>MARYURI AVENDAÑO BADILLO</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (LUIS EDUARDO OLIVEROS RAMIRES) vs Sofía (LUIS EDUARDO OLIVEROS RAMIREZ)</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (MARYURIAVENDAÑOBADILLO) vs Sofía (MARYURI AVENDAÑO BADILLO)</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>250188492</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>250188492</t>
+          <t>1020434371</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>NORA MARIA BLANDON SERNA</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>NORA MARIA BLANDON SERNA</t>
+          <t>LISSETHJOHANAMUÑOZMONTOYA</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>31642764</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>31642764</t>
+          <t>1023004785</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
+          <t>EDUARDRICARDOQUILISMALGALINDO</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>CC</t>
+          <t xml:space="preserve">TI </t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>31863992</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>31863992</t>
+          <t>1024483713</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>ALBA INES ZULETA JARAMILLO</t>
+          <t>JULY STEPHANIA VILLADA VARGAS</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3031278</v>
+        <v>3127639</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1151,7 +821,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -1166,88 +836,55 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>327311712</t>
+          <t>1026161730</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>327311712</t>
+          <t>1026161730</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>LORENATRUJILLORESTREPO</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
+          <t>LORENA TRUJILLO RESTREPO</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (LORENATRUJILLORESTREPO) vs Sofía (LORENA TRUJILLO RESTREPO)</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>36380685</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>36380685</t>
+          <t>1045688195</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
+          <t>LAURAESTEFANIAMIERBALLESTAS</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3031278</v>
+        <v>3127639</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1261,7 +898,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1276,143 +913,77 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>38553002</t>
+          <t>1058786387</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>38553002</t>
+          <t>1058786387</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>KARENSOFIACRUZSUAREZ</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>PAOLA ANDREA CASTILLO ALZATE</t>
+          <t>KAREN SOFIA CRUZ SUAREZ</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (KARENSOFIACRUZSUAREZ) vs Sofía (KAREN SOFIA CRUZ SUAREZ)</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>42057870</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>42057870</t>
+          <t>1075298940</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>MARTHA LUCIA ALZATE GOMEZ</t>
+          <t>DANNAVANESSATOVARBARRERA</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n">
-        <v>3031278</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>66655884</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>66655884</t>
+          <t>1084727175</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>MARIA DEL CARMEN CERON BEDOYA</t>
+          <t>NAYERLISDIAZBARRAZA</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3031278</v>
+        <v>3127639</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1426,7 +997,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1436,38 +1007,38 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>CC</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>66756576</t>
+          <t>1089000238</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>66756576</t>
+          <t>1089000238</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+          <t>LEONIZACOIMEOROBIO</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
+          <t>LEONIZA COIME OROBIO</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Tipo de Documento: Instructores (CC) vs Sofía (TI)</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (LEONIZACOIMEOROBIO) vs Sofía (LEONIZA COIME OROBIO)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3031278</v>
+        <v>3127639</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1481,7 +1052,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1496,27 +1067,258 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>66767235</t>
+          <t>1090513368</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>66767235</t>
+          <t>1090513368</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
+          <t>WILLIAMDAVIDVARGASNIÑO</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
+          <t>WILLIAM DAVID VARGAS NIÑO</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>VERDADERO</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (WILLIAMDAVIDVARGASNIÑO) vs Sofía (WILLIAM DAVID VARGAS NIÑO)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>3127639</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1098808954</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>1098808954</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CARLOSEDUARDOSOLANOBARRIOS</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>CARLOS EDUARDO SOLANO BARRIOS</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>FALSO - Discrepancia en Nombre: Instructores (CARLOSEDUARDOSOLANOBARRIOS) vs Sofía (CARLOS EDUARDO SOLANO BARRIOS)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>1115449528</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>MARIACAMILABERMUDEZMORENO</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>FALSO - Documento sólo en Instructores</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>1128055686</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>ALVARORAFAELMANJARREZPUCHE</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>FALSO - Documento sólo en Instructores</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3127639</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>1143859908</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>1143859908</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>YULIANDREACABALHILAMO</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>YULI ANDREA CABAL HILAMO</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>FALSO - Discrepancia en Nombre: Instructores (YULIANDREACABALHILAMO) vs Sofía (YULI ANDREA CABAL HILAMO)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3127639</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>1193114716</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>1193114716</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>ANGIEPAOLAMONTALVOBEJARANO</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>ANGIE PAOLA MONTALVO BEJARANO</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>FALSO - Discrepancia en Nombre: Instructores (ANGIEPAOLAMONTALVOBEJARANO) vs Sofía (ANGIE PAOLA MONTALVO BEJARANO)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>1193459571</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>SEBASTIANANDRESLUNAMORENO</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se hace el ajuste verdadero en consulta si el nombre consulta esta pegado
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -470,7 +470,7 @@
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="39" customWidth="1" min="9" max="9"/>
     <col width="31" customWidth="1" min="10" max="10"/>
-    <col width="116" customWidth="1" min="11" max="11"/>
+    <col width="107" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -735,7 +735,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (MARYURIAVENDAÑOBADILLO) vs Sofía (MARYURI AVENDAÑO BADILLO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (LORENATRUJILLORESTREPO) vs Sofía (LORENA TRUJILLO RESTREPO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -933,7 +933,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (KARENSOFIACRUZSUAREZ) vs Sofía (KAREN SOFIA CRUZ SUAREZ)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1032,7 +1032,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (LEONIZACOIMEOROBIO) vs Sofía (LEONIZA COIME OROBIO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (WILLIAMDAVIDVARGASNIÑO) vs Sofía (WILLIAM DAVID VARGAS NIÑO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (CARLOSEDUARDOSOLANOBARRIOS) vs Sofía (CARLOS EDUARDO SOLANO BARRIOS)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>YULIANDREACABALHILAMO</t>
+          <t>YULIANDREACABALHILAMOS</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (YULIANDREACABALHILAMO) vs Sofía (YULI ANDREA CABAL HILAMO)</t>
+          <t>FALSO - Discrepancia en Nombre: Instructores (YULIANDREACABALHILAMOS) vs Sofía (YULI ANDREA CABAL HILAMO)</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (ANGIEPAOLAMONTALVOBEJARANO) vs Sofía (ANGIE PAOLA MONTALVO BEJARANO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se hace que aparezca el codigo de la ficha cuando se ingresa el archivo
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -470,7 +470,7 @@
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="39" customWidth="1" min="9" max="9"/>
     <col width="31" customWidth="1" min="10" max="10"/>
-    <col width="107" customWidth="1" min="11" max="11"/>
+    <col width="40" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>YULIANDREACABALHILAMOS</t>
+          <t>YULIANDREACABALHILAMO</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>FALSO - Discrepancia en Nombre: Instructores (YULIANDREACABALHILAMOS) vs Sofía (YULI ANDREA CABAL HILAMO)</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se acomodan los botones
</commit_message>
<xml_diff>
--- a/scac/BackEnd/resultado_validacion.xlsx
+++ b/scac/BackEnd/resultado_validacion.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,14 @@
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="16" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
-    <col width="71" customWidth="1" min="4" max="4"/>
+    <col width="41" customWidth="1" min="4" max="4"/>
     <col width="29" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
     <col width="28" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="39" customWidth="1" min="9" max="9"/>
-    <col width="31" customWidth="1" min="10" max="10"/>
-    <col width="40" customWidth="1" min="11" max="11"/>
+    <col width="36" customWidth="1" min="10" max="10"/>
+    <col width="14" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -531,162 +531,393 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>1001779425</t>
+          <t>1005551692</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1005551692</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>SEBASTIANJIMENEZMAGALLANES</t>
+          <t>ZOILALUZALVAREZCALDERON</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>ZOILA LUZ ALVAREZ CALDERON</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1002921910</t>
+          <t>1010141404</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1010141404</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>ESTEFANNYGISELLAMUÑOZBARCO</t>
+          <t>LIZETH VANESSA PEDREROS ARANGO</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>LIZETH VANESSA PEDREROS ARANGO</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>1003237027</t>
+          <t>1051821219</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1051821219</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>CLAUDIAELENARESTREPOARANGO</t>
+          <t>CLAUDIAPATRICIAGRAVIERCALDERON</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>CLAUDIA PATRICIA GRAVIER CALDERON</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1003244042</t>
+          <t>1116242829</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1116242829</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>DUBYSTATIANABLANQUICETTMEJIA</t>
+          <t>LAURAMARCELAQUINTEROSANCHEZ</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>LAURA MARCELA QUINTERO SANCHEZ</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1003764743</t>
+          <t>1130643841</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1130643841</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>NEWMANESTIBENESCOBARCERON</t>
+          <t>FABIOROBINSONMALDONADOORDOÑEZ</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>FABIO ROBINSON MALDONADO ORDOÑEZ</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1004999377</t>
+          <t>16698345</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>16698345</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>ALIXVALENTINAANGARITAANGARITA</t>
+          <t>OMARURIELPATIÑOTORRES</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>OMAR URIEL PATIÑO TORRES</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>1005870821</t>
+          <t>167393272</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>167393272</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>MICHAELSTEVENCAMACHOACEVEDO</t>
+          <t>JOAQUINBERNARDOLOPEZPEREA</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>JOAQUIN BERNARDO LOPEZ PEREA</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3127639</v>
+        <v>3031278</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -700,7 +931,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -715,22 +946,22 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>1007514084</t>
+          <t>18464762</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1007514084</t>
+          <t>18464762</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>MARYURIAVENDAÑOBADILLO</t>
+          <t>LUISEDUARDOOLIVEROSRAMIREZ</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>MARYURI AVENDAÑO BADILLO</t>
+          <t>LUIS EDUARDO OLIVEROS RAMIREZ</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -740,74 +971,173 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>1020434371</t>
+          <t>250188492</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>250188492</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>LISSETHJOHANAMUÑOZMONTOYA</t>
+          <t>NORAMARIABLANDONSERNA</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>NORA MARIA BLANDON SERNA</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1023004785</t>
+          <t>31642764</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>31642764</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>EDUARDRICARDOQUILISMALGALINDO</t>
+          <t>INGRIYEANAESCOBAR</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">INGRI YEANA ESCOBAR </t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">TI </t>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>CC</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>1024483713</t>
+          <t>31863992</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>31863992</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>JULY STEPHANIA VILLADA VARGAS</t>
+          <t>ALBAINESZULETAJARAMILLO</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>ALBA INES ZULETA JARAMILLO</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3127639</v>
+        <v>3031278</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -821,7 +1151,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -836,22 +1166,22 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1026161730</t>
+          <t>327311712</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>1026161730</t>
+          <t>327311712</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>LORENATRUJILLORESTREPO</t>
+          <t>ZAILANDELCARMENCALDERONLOCARNO</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>LORENA TRUJILLO RESTREPO</t>
+          <t>ZAILAN DEL CARMEN CALDERON LOCARNO</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
@@ -861,30 +1191,63 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>1045688195</t>
+          <t>36380685</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>36380685</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>LAURAESTEFANIAMIERBALLESTAS</t>
+          <t>GLORIAYENNYCASTILLOESPAÑA</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>GLORIA YENNY CASTILLO ESPAÑA</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3127639</v>
+        <v>3031278</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -898,7 +1261,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -913,22 +1276,22 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>1058786387</t>
+          <t>38553002</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>1058786387</t>
+          <t>38553002</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>KARENSOFIACRUZSUAREZ</t>
+          <t>PAOLAANDREACASTILLOALZATE</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>KAREN SOFIA CRUZ SUAREZ</t>
+          <t>PAOLA ANDREA CASTILLO ALZATE</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -938,52 +1301,118 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1075298940</t>
+          <t>42057870</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>42057870</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>DANNAVANESSATOVARBARRERA</t>
+          <t>MARTHALUCIAALZATEGOMEZ</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>MARTHA LUCIA ALZATE GOMEZ</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="n">
+        <v>3031278</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>COMPLEMENTARIA</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>CURSO ESPECIAL</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>CC</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>1084727175</t>
+          <t>66655884</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>66655884</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>NAYERLISDIAZBARRAZA</t>
+          <t>MARIADELCARMENCERONBEDOYA</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>MARIA DEL CARMEN CERON BEDOYA</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>FALSO - Documento sólo en Instructores</t>
+          <t>VERDADERO</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>3127639</v>
+        <v>3031278</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -997,7 +1426,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1007,27 +1436,27 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1089000238</t>
+          <t>66756576</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>1089000238</t>
+          <t>66756576</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>LEONIZACOIMEOROBIO</t>
+          <t>MARTHAISABELBENAVIDESACOSTA</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>LEONIZA COIME OROBIO</t>
+          <t>MARTHA ISABEL BENAVIDES ACOSTA</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1038,7 +1467,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>3127639</v>
+        <v>3031278</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1052,7 +1481,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
+          <t>ELABORACION DE PRODUCTOS DE REPOSTERIA.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1067,258 +1496,27 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>1090513368</t>
+          <t>66767235</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>1090513368</t>
+          <t>66767235</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>WILLIAMDAVIDVARGASNIÑO</t>
+          <t>CLAUDIAPATRICIAARCEESCOBAR</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>WILLIAM DAVID VARGAS NIÑO</t>
+          <t>CLAUDIA PATRICIA ARCE ESCOBAR</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>VERDADERO</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3127639</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>1098808954</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>1098808954</t>
-        </is>
-      </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>CARLOSEDUARDOSOLANOBARRIOS</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>CARLOS EDUARDO SOLANO BARRIOS</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>VERDADERO</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>1115449528</t>
-        </is>
-      </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>MARIACAMILABERMUDEZMORENO</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>FALSO - Documento sólo en Instructores</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>1128055686</t>
-        </is>
-      </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>ALVARORAFAELMANJARREZPUCHE</t>
-        </is>
-      </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>FALSO - Documento sólo en Instructores</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>3127639</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>1143859908</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>1143859908</t>
-        </is>
-      </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>YULIANDREACABALHILAMO</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>YULI ANDREA CABAL HILAMO</t>
-        </is>
-      </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>VERDADERO</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>3127639</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>COMPLEMENTARIA</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>CURSO ESPECIAL</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>FUNDAMENTOS DEL SISTEMA DE GESTION DE SEGURIDAD Y SALUD EN EL TRABAJO</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>1193114716</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>1193114716</t>
-        </is>
-      </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>ANGIEPAOLAMONTALVOBEJARANO</t>
-        </is>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>ANGIE PAOLA MONTALVO BEJARANO</t>
-        </is>
-      </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>VERDADERO</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>CC</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>1193459571</t>
-        </is>
-      </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>SEBASTIANANDRESLUNAMORENO</t>
-        </is>
-      </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>FALSO - Documento sólo en Instructores</t>
         </is>
       </c>
     </row>

</xml_diff>